<commit_message>
Merged clue players 1 into main
</commit_message>
<xml_diff>
--- a/data/ClueLayout.xlsx
+++ b/data/ClueLayout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10329"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lpisano/Documents/MAC/Mines/CSCI306/Workspace/ClueGame/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C32EEBF-FC67-6D47-885D-E493CDD307DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00DFCC9B-5A3B-C740-86CC-ECDC3C63E02D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="23260" windowHeight="12460" xr2:uid="{5BA9FB4D-EAB4-284D-BE57-DA3F9D1A048C}"/>
+    <workbookView xWindow="17140" yWindow="3360" windowWidth="14560" windowHeight="12460" activeTab="1" xr2:uid="{5BA9FB4D-EAB4-284D-BE57-DA3F9D1A048C}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -518,7 +518,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -527,7 +527,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -541,7 +541,7 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -565,9 +565,6 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1273,7 +1270,7 @@
   </sheetPr>
   <dimension ref="A1:AD30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="185" workbookViewId="0">
+    <sheetView zoomScaleNormal="185" workbookViewId="0">
       <selection activeCell="AC13" sqref="AC13"/>
     </sheetView>
   </sheetViews>
@@ -1712,7 +1709,7 @@
       <c r="AC5" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="AD5" s="40" t="s">
+      <c r="AD5" s="30" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1975,7 +1972,7 @@
       <c r="AC8" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="AD8" s="40" t="s">
+      <c r="AD8" s="30" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2064,7 +2061,7 @@
       <c r="AC9" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="AD9" s="40" t="s">
+      <c r="AD9" s="30" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2153,7 +2150,7 @@
       <c r="AC10" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="AD10" s="40" t="s">
+      <c r="AD10" s="30" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2242,7 +2239,7 @@
       <c r="AC11" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="AD11" s="40" t="s">
+      <c r="AD11" s="30" t="s">
         <v>61</v>
       </c>
     </row>
@@ -3896,8 +3893,8 @@
   </sheetPr>
   <dimension ref="A1:AC30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
+      <selection activeCell="V30" sqref="V30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>